<commit_message>
supply data for species report chart
</commit_message>
<xml_diff>
--- a/src/templates/scl_report_mvp.xlsx
+++ b/src/templates/scl_report_mvp.xlsx
@@ -13,6 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="country summary" sheetId="1" r:id="rId1"/>
+    <sheet name="landscapes over time" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,12 +25,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
   <si>
     <t>COUNTRY SUMMARY</t>
-  </si>
-  <si>
-    <t>Graph showing the area of tiger habitat (i.e. total land area) and area of TCLs (y) over time (x).  Title should include species, date and country</t>
   </si>
   <si>
     <t>Number of landscapes</t>
@@ -297,15 +295,34 @@
       <t xml:space="preserve"> (IUCN Classes I - VI), as defined in the World Database of Protected Areas as of the most recent version available for the report date</t>
     </r>
   </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Conservation Landscape (km2)</t>
+  </si>
+  <si>
+    <t>Restoration Landscape (km2)</t>
+  </si>
+  <si>
+    <t>Survey Landscape (km2)</t>
+  </si>
+  <si>
+    <t>Fragment Landscape (km2)</t>
+  </si>
+  <si>
+    <t>Total tiger habitat area</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -355,59 +372,10 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="2">
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -427,15 +395,15 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -445,24 +413,6 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -476,18 +426,19 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -505,6 +456,1241 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:strRef>
+          <c:f>'country summary'!$F$3</c:f>
+          <c:strCache>
+            <c:ptCount val="1"/>
+            <c:pt idx="0">
+              <c:v> habitat area as of  for </c:v>
+            </c:pt>
+          </c:strCache>
+        </c:strRef>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="6.8110912167763757E-2"/>
+          <c:y val="0.15687016964742734"/>
+          <c:w val="0.7319861409224484"/>
+          <c:h val="0.63304356629590741"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'landscapes over time'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Conservation Landscape (km2)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'landscapes over time'!$A$2:$A$6</c:f>
+              <c:numCache>
+                <c:formatCode>yyyy\-mm\-dd;@</c:formatCode>
+                <c:ptCount val="5"/>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'landscapes over time'!$B$2:$B$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-5974-4341-B097-90709C509E97}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'landscapes over time'!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total tiger habitat area</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'landscapes over time'!$A$2:$A$6</c:f>
+              <c:numCache>
+                <c:formatCode>yyyy\-mm\-dd;@</c:formatCode>
+                <c:ptCount val="5"/>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'landscapes over time'!$F$2:$F$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000A-5974-4341-B097-90709C509E97}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="472071256"/>
+        <c:axId val="472072240"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="1"/>
+                <c:order val="1"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'landscapes over time'!$C$1</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>Restoration Landscape (km2)</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="28575" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent2"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="circle"/>
+                  <c:size val="5"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent2"/>
+                    </a:solidFill>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="accent2"/>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
+                <c:cat>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'landscapes over time'!$A$2:$A$6</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>yyyy\-mm\-dd;@</c:formatCode>
+                      <c:ptCount val="5"/>
+                    </c:numCache>
+                  </c:numRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'landscapes over time'!$C$2:$C$6</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="5"/>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000007-5974-4341-B097-90709C509E97}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredLineSeries>
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="2"/>
+                <c:order val="2"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'landscapes over time'!$D$1</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>Survey Landscape (km2)</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="28575" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent3"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="circle"/>
+                  <c:size val="5"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent3"/>
+                    </a:solidFill>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="accent3"/>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
+                <c:cat>
+                  <c:numRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'landscapes over time'!$A$2:$A$6</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>yyyy\-mm\-dd;@</c:formatCode>
+                      <c:ptCount val="5"/>
+                    </c:numCache>
+                  </c:numRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'landscapes over time'!$D$2:$D$6</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="5"/>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000008-5974-4341-B097-90709C509E97}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredLineSeries>
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="3"/>
+                <c:order val="3"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'landscapes over time'!$E$1</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>Fragment Landscape (km2)</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="28575" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent4"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="circle"/>
+                  <c:size val="5"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent4"/>
+                    </a:solidFill>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="accent4"/>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
+                <c:cat>
+                  <c:numRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'landscapes over time'!$A$2:$A$6</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>yyyy\-mm\-dd;@</c:formatCode>
+                      <c:ptCount val="5"/>
+                    </c:numCache>
+                  </c:numRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'landscapes over time'!$E$2:$E$6</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="5"/>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000009-5974-4341-B097-90709C509E97}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredLineSeries>
+          </c:ext>
+        </c:extLst>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="472071256"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="yyyy\-mm\-dd;@" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="472072240"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="1"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="472072240"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="472071256"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.80421386753809143"/>
+          <c:y val="0.28549210084838844"/>
+          <c:w val="0.18755250356615"/>
+          <c:h val="0.30298870533474942"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>147636</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>642937</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>40481</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -770,7 +1956,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K21"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -780,149 +1966,87 @@
     <col min="2" max="4" width="14.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="F2" s="10" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="10"/>
+      <c r="F3" t="str">
+        <f>B3 &amp; " habitat area as of " &amp; B4 &amp; " for " &amp; B5</f>
+        <v xml:space="preserve"> habitat area as of  for </v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="11"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="12"/>
+    </row>
+    <row r="7" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
-      <c r="K2" s="12"/>
+      <c r="C7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" s="4"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" s="16"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
-      <c r="K3" s="15"/>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="13"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="4"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" s="17"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="14"/>
-      <c r="J4" s="14"/>
-      <c r="K4" s="15"/>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="13"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="4"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" s="18"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="14"/>
-      <c r="K5" s="15"/>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="13"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="4"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="F6" s="13"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="15"/>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A11" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="16"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="4"/>
     </row>
-    <row r="7" spans="1:11" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A7" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E7" s="4"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="14"/>
-      <c r="K7" s="15"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A8" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" s="19"/>
-      <c r="C8" s="20"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="14"/>
-      <c r="K8" s="15"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9" s="19"/>
-      <c r="C9" s="20"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="14"/>
-      <c r="K9" s="15"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" s="19"/>
-      <c r="C10" s="20"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="14"/>
-      <c r="K10" s="15"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A11" s="5" t="s">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
         <v>7</v>
-      </c>
-      <c r="B11" s="22"/>
-      <c r="C11" s="23"/>
-      <c r="D11" s="24"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
-      <c r="J11" s="14"/>
-      <c r="K11" s="15"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A12" t="s">
-        <v>8</v>
       </c>
       <c r="B12" s="9">
         <f>SUM(B8:B11)</f>
@@ -932,82 +2056,105 @@
         <f>SUM(C8:C11)</f>
         <v>0</v>
       </c>
-      <c r="D12" s="25"/>
+      <c r="D12" s="19"/>
       <c r="E12" s="4"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="14"/>
-      <c r="K12" s="15"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
       <c r="E13" s="4"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="14"/>
-      <c r="K13" s="15"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
       <c r="E14" s="4"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A16" t="s">
-        <v>22</v>
-      </c>
-      <c r="B16" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17" t="s">
         <v>11</v>
-      </c>
-      <c r="B17" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" t="s">
         <v>13</v>
-      </c>
-      <c r="B18" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" t="s">
         <v>15</v>
-      </c>
-      <c r="B19" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B21" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="F2:K13"/>
-  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="9.9296875" style="20" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A1" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
handle nonexistent landscapes, tweak excel, comment ee renewal temp
</commit_message>
<xml_diff>
--- a/src/templates/scl_report_mvp.xlsx
+++ b/src/templates/scl_report_mvp.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kfisher\Documents\Asia\TCL3\work\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kfisher\repos\scl\scl-api\src\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -646,6 +646,21 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2125,7 +2140,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F300"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2154,6 +2169,1800 @@
         <v>28</v>
       </c>
     </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="F2">
+        <f>SUM(B2:E2)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="F3">
+        <f t="shared" ref="F3:F66" si="0">SUM(B3:E3)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="F4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="F11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="F13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="F14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="F15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="F16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F23">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F24">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F29">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F31">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F32">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F33">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F34">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F36">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F37">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F38">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F39">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F40">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F41">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F42">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F43">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F44">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F45">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F46">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F47">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F48">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F49">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F50">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F51">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F52">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F53">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F54">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F55">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F56">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F57">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F58">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F59">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F60">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F61">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F62">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F63">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F64">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F65">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F66">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F67">
+        <f t="shared" ref="F67:F130" si="1">SUM(B67:E67)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F68">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F69">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F70">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F71">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F72">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F73">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F74">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F75">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F76">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F77">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F78">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F79">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F80">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F81">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F82">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F83">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F84">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F85">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F86">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F87">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F88">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F89">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F90">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F91">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F92">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F93">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F94">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F95">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F96">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F97">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F98">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F99">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F100">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F101">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F102">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F103">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F104">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F105">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F106">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F107">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F108">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F109">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F110">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F111">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F112">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F113">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F114">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F115">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F116">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F117">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F118">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F119">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F120">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F121">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F122">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F123">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F124">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F125">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F126">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F127">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F128">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F129">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F130">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F131">
+        <f t="shared" ref="F131:F194" si="2">SUM(B131:E131)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F132">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F133">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F134">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F135">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F136">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F137">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F138">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F139">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F140">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F141">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F142">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F143">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F144">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="145" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F145">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F146">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F147">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="148" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F148">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="149" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F149">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="150" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F150">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F151">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="152" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F152">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="153" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F153">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="154" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F154">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="155" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F155">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="156" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F156">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="157" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F157">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="158" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F158">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="159" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F159">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="160" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F160">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="161" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F161">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="162" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F162">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="163" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F163">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="164" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F164">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="165" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F165">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="166" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F166">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="167" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F167">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="168" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F168">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="169" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F169">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="170" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F170">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="171" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F171">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="172" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F172">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="173" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F173">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="174" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F174">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="175" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F175">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="176" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F176">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="177" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F177">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="178" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F178">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="179" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F179">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="180" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F180">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="181" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F181">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="182" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F182">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="183" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F183">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="184" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F184">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="185" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F185">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="186" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F186">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="187" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F187">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="188" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F188">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="189" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F189">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="190" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F190">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="191" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F191">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="192" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F192">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="193" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F193">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="194" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F194">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="195" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F195">
+        <f t="shared" ref="F195:F258" si="3">SUM(B195:E195)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="196" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F196">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="197" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F197">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="198" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F198">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="199" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F199">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="200" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F200">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="201" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F201">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="202" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F202">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="203" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F203">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="204" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F204">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="205" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F205">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="206" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F206">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="207" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F207">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="208" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F208">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="209" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F209">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="210" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F210">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="211" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F211">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="212" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F212">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="213" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F213">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="214" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F214">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="215" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F215">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="216" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F216">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="217" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F217">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="218" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F218">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="219" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F219">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="220" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F220">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="221" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F221">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="222" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F222">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="223" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F223">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="224" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F224">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="225" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F225">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="226" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F226">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="227" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F227">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="228" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F228">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="229" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F229">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="230" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F230">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="231" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F231">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="232" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F232">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="233" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F233">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="234" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F234">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="235" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F235">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="236" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F236">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="237" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F237">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="238" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F238">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="239" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F239">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="240" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F240">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="241" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F241">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="242" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F242">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="243" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F243">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="244" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F244">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="245" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F245">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="246" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F246">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="247" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F247">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="248" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F248">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="249" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F249">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="250" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F250">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="251" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F251">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="252" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F252">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="253" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F253">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="254" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F254">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="255" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F255">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="256" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F256">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="257" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F257">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="258" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F258">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="259" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F259">
+        <f t="shared" ref="F259:F270" si="4">SUM(B259:E259)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="260" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F260">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="261" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F261">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="262" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F262">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="263" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F263">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="264" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F264">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="265" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F265">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="266" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F266">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="267" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F267">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="268" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F268">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="269" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F269">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="270" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F270">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="271" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F271">
+        <f>SUM(B271:E271)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="272" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F272">
+        <f t="shared" ref="F272:F300" si="5">SUM(B272:E272)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="273" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F273">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="274" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F274">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="275" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F275">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="276" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F276">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="277" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F277">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="278" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F278">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="279" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F279">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="280" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F280">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="281" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F281">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="282" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F282">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="283" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F283">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="284" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F284">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="285" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F285">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="286" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F286">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="287" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F287">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="288" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F288">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="289" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F289">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="290" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F290">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="291" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F291">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="292" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F292">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="293" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F293">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="294" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F294">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="295" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F295">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="296" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F296">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="297" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F297">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="298" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F298">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="299" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F299">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="300" spans="6:6" x14ac:dyDescent="0.45">
+      <c r="F300">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Country and Global excel reports
</commit_message>
<xml_diff>
--- a/src/templates/scl_report_mvp.xlsx
+++ b/src/templates/scl_report_mvp.xlsx
@@ -10,6 +10,7 @@
   <sheets>
     <sheet name="country summary" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="landscapes over time" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="aggregated" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -21,42 +22,42 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="55">
-  <si>
-    <t xml:space="preserve">&lt;country&gt; | Global Summary</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Date generated: &lt;date&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Species: &lt;species&gt;</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="64">
+  <si>
+    <t xml:space="preserve">&lt;Country&gt; Summary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date generated: &lt;today&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Species: &lt;Species&gt; (&lt;specieslatin&gt;)</t>
   </si>
   <si>
     <t xml:space="preserve">Date: &lt;date&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;country&gt; | Global habitat Area for &lt;species&gt; over time</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;country&gt; | Global habitat Area for &lt;species&gt; in &lt;date&gt;</t>
+    <t xml:space="preserve">&lt;Country&gt; habitat area for &lt;species&gt;s over time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;Country&gt; habitat area for &lt;species&gt;s (&lt;specieslatin&gt;) in &lt;date&gt;</t>
   </si>
   <si>
     <t xml:space="preserve">Habitat Area</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;species&gt; Landscape Types</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Number of landscapes</t>
+    <t xml:space="preserve">&lt;Species&gt; Landscape Types</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of Landscapes</t>
   </si>
   <si>
     <t xml:space="preserve">Habitat Area (km2)</t>
   </si>
   <si>
-    <t xml:space="preserve">% Protected</t>
-  </si>
-  <si>
-    <t xml:space="preserve">% KBA</t>
+    <t xml:space="preserve">% Protected, of Landscape Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">% KBA, of Landscape Type</t>
   </si>
   <si>
     <t xml:space="preserve">% Total Habitat</t>
@@ -68,7 +69,7 @@
     <t xml:space="preserve">Known Occupied Habitat</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;species&gt; Conservation Landscapes</t>
+    <t xml:space="preserve">&lt;Species&gt; Conservation Landscapes</t>
   </si>
   <si>
     <t xml:space="preserve">xx</t>
@@ -83,10 +84,10 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t xml:space="preserve">Fragments with &lt;species&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total occupied habitat</t>
+    <t xml:space="preserve">Fragments with &lt;Species&gt;s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total Occupied Habitat</t>
   </si>
   <si>
     <t xml:space="preserve">Available Habitat</t>
@@ -104,28 +105,22 @@
     <t xml:space="preserve">Fragments for Restoration</t>
   </si>
   <si>
-    <t xml:space="preserve">Total available habitat</t>
+    <t xml:space="preserve">Total Available Habitat</t>
   </si>
   <si>
     <t xml:space="preserve">Total Habitat</t>
   </si>
   <si>
-    <t xml:space="preserve">Available + occupied habitats</t>
+    <t xml:space="preserve">Available + Occupied Habitats</t>
   </si>
   <si>
     <t xml:space="preserve">Total Indigenous Range</t>
   </si>
   <si>
-    <t xml:space="preserve">--</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ratio of occupied / available habitat: x.xx</t>
-  </si>
-  <si>
     <t xml:space="preserve">Definitions</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;species&gt; Conservation Landscape</t>
+    <t xml:space="preserve">&lt;Species&gt; Conservation Landscape</t>
   </si>
   <si>
     <r>
@@ -161,7 +156,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Restoration landscape</t>
+    <t xml:space="preserve">Restoration Landscape</t>
   </si>
   <si>
     <r>
@@ -197,7 +192,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Survey landscape</t>
+    <t xml:space="preserve">Survey Landscape</t>
   </si>
   <si>
     <r>
@@ -233,7 +228,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Fragment with &lt;species&gt;</t>
+    <t xml:space="preserve">Fragment with &lt;Species&gt;</t>
   </si>
   <si>
     <r>
@@ -259,7 +254,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Fragment for survey</t>
+    <t xml:space="preserve">Fragment for Survey</t>
   </si>
   <si>
     <r>
@@ -285,7 +280,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Fragment for restoration</t>
+    <t xml:space="preserve">Fragment for Restoration</t>
   </si>
   <si>
     <r>
@@ -380,34 +375,68 @@
     <t xml:space="preserve">The area of the landscape type as a percentage of all habitat in the country or globally</t>
   </si>
   <si>
-    <t xml:space="preserve">The area of the landscape type as a percentage of all of the indigenous range for &lt;species&gt; in the country or globally</t>
+    <t xml:space="preserve">The area of the landscape type as a percentage of all of the indigenous range for &lt;species&gt;s  in the country or globally</t>
   </si>
   <si>
     <t xml:space="preserve">date</t>
   </si>
   <si>
+    <t xml:space="preserve">country_code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">country_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">landscape_type</t>
+  </si>
+  <si>
     <t xml:space="preserve">landscape_id</t>
   </si>
   <si>
-    <t xml:space="preserve">landscape_type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">landscape_area</t>
-  </si>
-  <si>
-    <t xml:space="preserve">biome_areas</t>
+    <t xml:space="preserve">landscape_habitat_area</t>
+  </si>
+  <si>
+    <t xml:space="preserve">biome_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">biome_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">biome_habitat_area</t>
+  </si>
+  <si>
+    <t xml:space="preserve">biome_habitat_area_protected</t>
+  </si>
+  <si>
+    <t xml:space="preserve">biome_habitat_area_key_biodiversity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">biome_protected_areas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">biome_key_biodiversity_areas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">habitat_area</t>
+  </si>
+  <si>
+    <t xml:space="preserve">habitat_area_protected</t>
+  </si>
+  <si>
+    <t xml:space="preserve">habitat_area_key_biodiversity</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
-    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="166" formatCode="#,##0"/>
+    <numFmt numFmtId="167" formatCode="yyyy/mm/dd;@"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -446,27 +475,48 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD8D8D8"/>
+        <bgColor rgb="FFC0C0C0"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="thin"/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="thin"/>
+      <top/>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
   </borders>
@@ -495,7 +545,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="17">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -516,10 +566,38 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -528,11 +606,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -545,6 +623,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFD8D8D8"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -559,9 +697,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>818640</xdr:colOff>
+      <xdr:colOff>296640</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>26640</xdr:rowOff>
+      <xdr:rowOff>24120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -575,7 +713,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="1270800"/>
-          <a:ext cx="7699320" cy="4636440"/>
+          <a:ext cx="7696800" cy="4633920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -598,17 +736,17 @@
   <dimension ref="A1:H63"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K13" activeCellId="0" sqref="K13"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="32.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="38.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="7.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="9.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="14.66"/>
   </cols>
@@ -732,12 +870,12 @@
     <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="3"/>
     </row>
-    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="4" t="s">
         <v>6</v>
       </c>
@@ -753,7 +891,7 @@
       <c r="E37" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F37" s="4" t="s">
+      <c r="F37" s="5" t="s">
         <v>11</v>
       </c>
       <c r="G37" s="4" t="s">
@@ -764,327 +902,316 @@
       </c>
     </row>
     <row r="38" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="5" t="s">
+      <c r="A38" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B38" s="5" t="s">
+      <c r="B38" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C38" s="5" t="s">
+      <c r="C38" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D38" s="5" t="s">
+      <c r="D38" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E38" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F38" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G38" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="H38" s="5" t="s">
+      <c r="E38" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F38" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G38" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H38" s="6" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="5" t="s">
+      <c r="A39" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B39" s="5" t="s">
+      <c r="B39" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C39" s="5" t="s">
+      <c r="C39" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D39" s="5" t="s">
+      <c r="D39" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E39" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F39" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G39" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="H39" s="5" t="s">
+      <c r="E39" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F39" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G39" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H39" s="6" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="5" t="s">
+      <c r="A40" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B40" s="5" t="s">
+      <c r="B40" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C40" s="5" t="s">
+      <c r="C40" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D40" s="5" t="s">
+      <c r="D40" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="E40" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F40" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G40" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="H40" s="5" t="s">
+      <c r="E40" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="F40" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="G40" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="H40" s="10" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="5" t="s">
+      <c r="A41" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B41" s="5" t="s">
+      <c r="B41" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C41" s="5" t="s">
+      <c r="C41" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D41" s="5" t="s">
+      <c r="D41" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E41" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F41" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G41" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="H41" s="5" t="s">
+      <c r="E41" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F41" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G41" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H41" s="6" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="5" t="s">
+      <c r="A42" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B42" s="5" t="s">
+      <c r="B42" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C42" s="5" t="s">
+      <c r="C42" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D42" s="5" t="s">
+      <c r="D42" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E42" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F42" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G42" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="H42" s="5" t="s">
+      <c r="E42" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F42" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G42" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H42" s="6" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="5" t="s">
+      <c r="A43" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B43" s="5" t="s">
+      <c r="B43" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C43" s="5" t="s">
+      <c r="C43" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D43" s="5" t="s">
+      <c r="D43" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E43" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F43" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G43" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="H43" s="5" t="s">
+      <c r="E43" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F43" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G43" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H43" s="6" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="5" t="s">
+      <c r="A44" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B44" s="5" t="s">
+      <c r="B44" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C44" s="5" t="s">
+      <c r="C44" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D44" s="5" t="s">
+      <c r="D44" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E44" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F44" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G44" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="H44" s="5" t="s">
+      <c r="E44" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F44" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G44" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H44" s="6" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="5" t="s">
+      <c r="A45" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B45" s="5" t="s">
+      <c r="B45" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="C45" s="5" t="s">
+      <c r="C45" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D45" s="5" t="s">
+      <c r="D45" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="E45" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F45" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G45" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="H45" s="5" t="s">
+      <c r="E45" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="F45" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="G45" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="H45" s="10" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="5" t="s">
+      <c r="A46" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B46" s="5" t="s">
+      <c r="B46" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C46" s="5" t="s">
+      <c r="C46" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D46" s="5" t="s">
+      <c r="D46" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E46" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F46" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G46" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="H46" s="5" t="s">
+      <c r="E46" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F46" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G46" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H46" s="6" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="5" t="s">
+      <c r="A47" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B47" s="5" t="s">
+      <c r="B47" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C47" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D47" s="5" t="s">
+      <c r="C47" s="6"/>
+      <c r="D47" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E47" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F47" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G47" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="H47" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="0" t="s">
-        <v>32</v>
-      </c>
+      <c r="E47" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F47" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G47" s="6"/>
+      <c r="H47" s="6"/>
     </row>
     <row r="51" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B51" s="6"/>
-      <c r="C51" s="6"/>
-      <c r="D51" s="6"/>
-      <c r="E51" s="7"/>
+      <c r="B51" s="13"/>
+      <c r="C51" s="13"/>
+      <c r="D51" s="13"/>
+      <c r="E51" s="14"/>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B53" s="0" t="s">
         <v>33</v>
-      </c>
-    </row>
-    <row r="53" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B53" s="0" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B55" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="B55" s="0" t="s">
+      <c r="B56" s="0" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="5" t="s">
+    <row r="57" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="B56" s="0" t="s">
+      <c r="B57" s="0" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="5" t="s">
+    <row r="58" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B57" s="0" t="s">
+      <c r="B58" s="0" t="s">
         <v>43</v>
-      </c>
-    </row>
-    <row r="58" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B58" s="0" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1092,7 +1219,7 @@
         <v>10</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1100,23 +1227,23 @@
         <v>11</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="B62" s="8" t="s">
-        <v>48</v>
+      <c r="B62" s="15" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="B63" s="8" t="s">
-        <v>49</v>
+      <c r="B63" s="15" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -1136,43 +1263,71 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E1048576"/>
+  <dimension ref="A1:M1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="9" width="9.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.47"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="26.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="22.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="24.47"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="21.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="16" width="9.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="16" width="15.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="16" width="14.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="22.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="12.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="21.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="27.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="31.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="32.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="27.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="26.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="9.14"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="9" t="s">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="D1" s="0" t="s">
         <v>51</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="E1" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="F1" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="G1" s="0" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="H1" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="K1" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="L1" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="M1" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -1182,4 +1337,51 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="21.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="26.46"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>63</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>